<commit_message>
DA17 | Day 4
</commit_message>
<xml_diff>
--- a/Batch/17/Day_4_Logical.xlsx
+++ b/Batch/17/Day_4_Logical.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28422"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Acciojob\Modules\Excel\Batch\15\Curriculum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ac217573afc2a6e8/Work/Acciojob/Modules/Excel/Batch/17/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E198994-0BA2-421F-9F5F-8C5F75355733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{6E198994-0BA2-421F-9F5F-8C5F75355733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82A724DA-D7EF-4A41-B5A9-FFDCD3BE1C15}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3830" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3827" uniqueCount="323">
   <si>
     <t>Data Used in Formula</t>
   </si>
@@ -1710,19 +1710,10 @@
     <t>10. Create a formula using ISBLANK to identify which employees do not have a performance rating recorded.</t>
   </si>
   <si>
-    <t>Quantity</t>
+    <t>=IF(C14&gt;89,"A",IF(C14&gt;79,"B",if(C14&gt;69,"C",IF(C14&gt;59,"D","F"))))</t>
   </si>
   <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>Price/Item</t>
-  </si>
-  <si>
-    <t>Price /Item</t>
-  </si>
-  <si>
-    <t>=IF(C14&gt;89,"A",IF(C14&gt;79,"B",if(C14&gt;69,"C",if(C14&gt;59,"D","F"))))</t>
+    <t>=10/0</t>
   </si>
 </sst>
 </file>
@@ -1811,7 +1802,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1828,6 +1819,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFDE9D9"/>
         <bgColor rgb="FFFDE9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1975,7 +1972,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2064,6 +2061,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2432,308 +2432,7 @@
     </xdr:pic>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>972951</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>18476</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1982113</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>74665</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="30" name="Ink 29">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F19CC4F3-5D44-FEAC-CE11-04B2A3608D0E}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="4204882" y="754200"/>
-            <a:ext cx="1004400" cy="240120"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="30" name="Ink 29">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F19CC4F3-5D44-FEAC-CE11-04B2A3608D0E}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="4198760" y="748080"/>
-              <a:ext cx="1016644" cy="252360"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>915368</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>162447</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>752631</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>151758</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="31" name="Ink 30">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFEB85BA-0A90-B6CB-E6EC-A354CC5E2238}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="3109402" y="714240"/>
-            <a:ext cx="875160" cy="173242"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="31" name="Ink 30">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFEB85BA-0A90-B6CB-E6EC-A354CC5E2238}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="3103252" y="708117"/>
-              <a:ext cx="887461" cy="185488"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>77206</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>181527</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>751208</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>162918</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="32" name="Ink 31">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{505A8DF7-0C9C-6F36-A292-1633C635B501}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="2271240" y="733320"/>
-            <a:ext cx="674002" cy="165322"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="32" name="Ink 31">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{505A8DF7-0C9C-6F36-A292-1633C635B501}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2265119" y="727210"/>
-              <a:ext cx="686243" cy="177541"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2024-12-29T17:24:42.614"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-      <inkml:brushProperty name="color" value="#004F8B"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 272 8708,'0'0'9076,"0"-22"-8964,48 10 80,6-1 16,5-2-112,0 3-64,-10 3-32,5-4-48,-11 4-368,-11 0-912,-5 0-1073,-16 6-3154,-11-4 289</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="215.31">246 99 2049,'0'0'9482,"4"-3"-9346,1 1-124,0-1 0,0 1-1,0 0 1,0 1 0,0-1 0,1 1 0,-1 0 0,1 0 0,-1 1 0,1 0 0,-1-1 0,1 2 0,-1-1-1,0 1 1,9 2 0,-11-3 38,1 1-1,-1 0 1,1-1-1,-1 2 1,0-1-1,0 0 1,0 1-1,1-1 0,-1 1 1,-1 0-1,1 0 1,0 0-1,0 0 1,-1 1-1,1-1 1,-1 1-1,0-1 1,0 1-1,0 0 1,0 0-1,0 0 0,0 0 1,-1 0-1,0 1 1,0-1-1,2 6 1,-3-4 157,0 0 1,0-1 0,0 1 0,-1 0-1,0 0 1,0-1 0,0 1-1,0 0 1,-1-1 0,0 1 0,0-1-1,0 0 1,0 1 0,-1-1-1,0 0 1,1-1 0,-1 1 0,-6 5-1,-8 7 97,-1 0 0,-34 23 0,-13 12-566,39-29-2087,9-10-2043,-5-2-4607</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1051.45">743 40 5843,'0'0'10314,"0"-5"-9303,0-18-219,0 18-328,0 9-287,-4 89-55,-19 106 1,18-103 48,5-95-173,1 0 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1-1 0,0 1 1,-1-1-1,1 1 0,0-1 0,0 1 0,-1-1 0,1 0 0,0 0 0,0 1 0,0-1 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,2 0 0,31-1-49,-26 1 59,12-2 9,0-1 1,0 0-1,-1-2 0,1 0 0,-1-1 1,31-15-1,37-11-1787,-57 22-629,-9 2-2066,-10 5 7</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1456.5">1211 173 4674,'0'0'8463,"-9"-3"-7514,-29-9-279,37 12-628,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 1 1,0-1 0,-1 1-1,1-1 1,-1 1-1,1 0 1,0-1-1,-1 1 1,1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 1-1,0-1 1,1 0 0,-1 1-1,0 1 1,-17 41 678,17-41-678,0 0-28,-1-1 0,1 1 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,0-1 0,0 1 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0-1,1 3 1,-1-4-6,1 0 0,0-1 0,-1 0 0,1 1 0,0-1 0,0 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,0-1 0,0 1 0,1 0 0,-1-1 0,0 0 0,0 1-1,0-1 1,0 0 0,0 0 0,1 0 0,2-1 0,2 1 8,0 0 1,0-1-1,0 0 1,0 0-1,0-1 1,0 0-1,0 0 0,0 0 1,-1-1-1,1 0 1,9-6-1,-13 7-5,0-1-1,0 1 1,1-1-1,-2 0 0,1 0 1,0 0-1,0-1 1,-1 1-1,0 0 1,0-1-1,0 0 0,0 1 1,0-1-1,-1 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,-1 0-1,0-5 1,-1 8-7,0-1 0,1 1 0,-1 0 0,-1-1 1,1 1-1,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 1,-1 0-1,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 1,-1 1-1,1 0 0,-1-1 0,0 1 0,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,-2 1 0,-3-1-49,1 0-1,-1 0 0,1 1 1,-1-1-1,1 2 1,-11 2-1,15-3-61,0 0 0,0 0 0,0 1 1,1-1-1,-1 0 0,0 1 0,0 0 0,1-1 0,-1 1 0,1 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 0,-1 2 0,-3 26-8161,5-24 3306</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1830.47">1491 188 224,'0'0'12062,"-8"8"-10830,8-8-1227,-5 4 141,1 1 0,-1 0 1,1 0-1,0 1 0,0-1 0,0 1 0,1 0 0,0 0 0,0 0 0,0 0 1,1 0-1,0 1 0,1-1 0,-1 1 0,1-1 0,-1 10 0,3-14-136,-1-1-1,0 0 1,1 1-1,-1-1 1,0 0-1,1 1 1,0-1-1,-1 0 1,1 0-1,0 1 1,0-1 0,-1 0-1,1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,0-1-1,0 1 1,0 0-1,1-1 1,-1 1-1,0-1 1,1 1-1,-1-1 1,1 1-1,-1-1 1,0 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,0 0 1,1 0-1,-1-1 1,1 1-1,-1 0 1,3-2-1,-2 2 31,1 0 0,-1-1 0,1 1-1,-1-1 1,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0-1,0-1 1,0 1 0,0-1-1,0 1 1,0-1 0,0 0-1,0 0 1,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0 0,0 0-1,0-1 1,0 1 0,1-3-1,-1 2-30,0 0 1,-1 0-1,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 1,-1 0-1,1 0 0,-1 0 0,0 0 0,0 0 0,0 1 0,0-1 0,-1 0 1,1 1-1,-1-1 0,1 1 0,-1-1 0,0 1 0,0 0 0,0-1 0,0 1 1,0 0-1,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,0 1 0,1 0 1,-1 0-1,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0 0 0,0 0 1,0-1-1,0 2 0,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,-2 1 1,4-2-323,0 1 1,1 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,0 0 0,0-1 0,0 1-1,-1 0 1,1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0-1 0,0 1 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,8 4-6619</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1922.62">1478 188 5843</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2323.72">1478 188 5843,'138'-105'2606,"-134"103"-2141,0-1 0,-1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0-1 0,2-4 0,-8 16 4214,6 60-4080,3-1 1,18 86-1,-22-145-753,0 0 0,0 0-1,1 1 1,0-1 0,0-1-1,1 1 1,0 0 0,8 10 0,-10-16-98,-1 0 1,1 1 0,0-1 0,1 0 0,-1 0-1,0-1 1,1 1 0,-1 0 0,1-1-1,-1 1 1,1-1 0,0 0 0,-1 0 0,1 0-1,0 0 1,0-1 0,0 1 0,0-1 0,0 0-1,0 1 1,-1-1 0,1-1 0,0 1-1,0 0 1,0-1 0,0 1 0,3-2 0,-4 1 46,1-1 1,0 1 0,0-1 0,-1 0 0,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 0-1,-1 0 1,0 0 0,0 1 0,0-1 0,0 0 0,0-4 0,2-5 368,-1 0 0,0-1 0,0-22 1,-2-1 1615,0 11 2893,-9 24-1782,-25 5-2228,14 7-606,1 1 1,0 1-1,1 1 0,0 1 1,-16 18-1,25-22 377,22-8 87,-1-2-587,176 15-782,-61-13-6380,-94-3 1996</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2654.1">2144 219 6259,'0'0'8561,"34"55"-6760,-30-51-1750,0 0-1,1 0 1,0-1 0,0 1 0,0-1 0,0 0-1,0-1 1,1 1 0,-1-1 0,1 0-1,-1 0 1,1-1 0,0 0 0,7 1-1,-10-1 0,0-1-1,0 1 0,0-1 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,1-1 0,-1 1 0,-1-1 1,1 0-1,0 0 0,0 0 0,0 0 0,0-1 0,-1 1 1,1-1-1,0 1 0,-1-1 0,0 0 0,1 0 1,-1 0-1,0-1 0,0 1 0,0 0 0,0-1 0,1-3 1,0-1 101,0 0 1,-1 0 0,-1 0 0,1 0 0,-1-1-1,0 1 1,-1-1 0,0-7 0,0 13-194,0 1 1,0-1 0,0 0-1,0 0 1,-1 1-1,1-1 1,0 0 0,-1 0-1,0 1 1,1-1-1,-1 0 1,0 1 0,0-1-1,0 1 1,0-1-1,0 1 1,0 0 0,0-1-1,-1 1 1,1 0-1,0 0 1,-1 0 0,1 0-1,-1 0 1,0 0 0,1 0-1,-1 0 1,1 1-1,-1-1 1,0 0 0,0 1-1,1 0 1,-1-1-1,0 1 1,0 0 0,-2 0-1,3 9-5835,1-3 1131</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2906.65">2478 22 1153,'0'0'15084,"0"-6"-14132,0-9-717,2 23 16,3 46 351,-1-5 130,16 339 367,-19-222-7411,6-170-1327,8-22 2939</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3141.53">2571 452 2673,'0'-19'2014,"-1"-13"-1348,0-11 1242,3-45 0,-2 79-1513,1-1 0,0 1 0,1-1 0,0 1 1,0 0-1,1 0 0,0 0 0,1 0 0,0 0 0,0 1 0,9-13 0,-9 17-288,-1 1-1,1-1 0,0 1 0,0 0 0,0 1 1,1-1-1,-1 1 0,1-1 0,-1 1 1,1 0-1,0 1 0,0-1 0,6 0 1,66-3 1331,-72 5-1309,-4 0-93,0 0-1,1 0 1,-1 0-1,0 0 0,0 1 1,1-1-1,-1 0 1,0 1-1,0-1 1,0 1-1,0-1 1,1 1-1,-1 0 1,0-1-1,0 1 1,0 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,-1 0-1,1 0 0,-1 0 1,1 1-1,-1-1 1,0 0-1,0 0 1,1 1-1,-1-1 1,0 0-1,0 0 1,0 1-1,0-1 1,-1 2-1,1 0 43,0 1-1,-1-1 0,1 1 1,-1-1-1,0 0 1,0 1-1,-1-1 0,1 0 1,0 0-1,-1 0 0,0 0 1,0 0-1,0 0 1,-2 2-1,-8 5 43,1-1 0,-1-1-1,-1 0 1,0-1 0,0 0 0,-23 8 0,-88 22-2301,85-30-1186,-3-6-2825</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2024-12-29T17:24:39.662"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-      <inkml:brushProperty name="color" value="#004F8B"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">43 174 2209,'0'0'10133,"0"13"-9498,1 38 787,-2 73 340,0-112-1687,0 0 0,-1 0 1,-1 0-1,0 0 0,-1-1 0,0 1 0,-10 20 0,14-32-72,0-1 0,0 1 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,-1-1 1,1 1 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0-1 0,-1 1-1,1 0 1,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 1 0,0-1 0,-1 0 0,1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 1-1,0-1 1,-4-23-49,3-28-157,1 50 203,0-19-162,1-1 1,1 0-1,1 0 1,1 0 0,0 1-1,2 0 1,0 0-1,2 0 1,13-26 0,-20 44 162,-1 1 0,1-1 0,0 0 1,1 1-1,-1-1 0,0 1 1,0-1-1,0 1 0,1 0 0,-1 0 1,1-1-1,-1 1 0,1 0 1,0 0-1,-1 0 0,1 1 0,0-1 1,0 0-1,-1 1 0,1-1 1,0 1-1,0-1 0,0 1 0,0 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0 0 0,0 1 0,0-1 1,0 0-1,0 1 0,-1 0 1,1-1-1,0 1 0,0 0 0,-1 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 1 0,1 2 1,8 5 121,-1 2 1,0-1 0,-1 1 0,11 17 0,-20-28-121,11 16-74,-1 1 0,-1 0-1,-1 0 1,-1 1 0,0 0 0,-1 0 0,4 21-1,-2 33-7036,-8-52 833</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="202.57">52 349 4306,'0'0'7187,"37"-62"-7251,-4 53-112,4 3-512,-10 3-465,5 0-607,-15 3-754,4 0-127</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="525.52">321 244 1809,'0'0'10650,"2"3"-10322,5 6 41,-1 1 0,0 0 0,-1-1-1,8 21 1,-10-21-272,0 0-1,1-1 1,0 0-1,0 0 1,1 0-1,0 0 1,1-1-1,-1 0 1,1 0-1,13 11 1,-18-16-75,1-1 1,0 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,1 0-1,-1-1 0,0 1 1,0-1-1,0 1 1,0-1-1,0 0 1,4 0-1,-5 0 26,0-1-1,0 1 0,0 0 0,0-1 1,0 1-1,0-1 0,0 0 0,0 1 0,0-1 1,0 0-1,0 0 0,0 0 0,0 1 1,0-1-1,-1 0 0,1 0 0,0 0 0,-1 0 1,1 0-1,0-2 0,2-6 249,0 0-1,-1 0 1,-1 0-1,1-1 1,-1-16 0,3-5-623,-4 29 198,0 1-1,0 0 1,1 0 0,-1 0-1,1 0 1,-1 0-1,1 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,0 0-1,-1 0 1,1 0-1,0 0 1,0 1 0,0-1-1,0 0 1,0 1-1,0-1 1,0 0 0,1 1-1,-1 0 1,0-1 0,0 1-1,1-1 1,35 0-6269,-21 2 5143,15-1-2200</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1074.35">839 265 688,'0'0'10282,"-17"-8"-8958,-55-25-81,70 32-1204,-1-1 1,0 1-1,0 0 0,0 0 1,0 0-1,0 1 0,-1-1 1,1 1-1,0 0 0,0 0 1,0 0-1,0 0 1,-1 0-1,1 1 0,0-1 1,0 1-1,0 0 0,0 0 1,0 0-1,0 0 0,0 1 1,1-1-1,-1 1 0,0-1 1,1 1-1,-1 0 1,1 0-1,0 1 0,-1-1 1,1 0-1,0 1 0,0-1 1,1 1-1,-1-1 0,-2 7 1,1-3-26,0 1 0,0 0 1,1 0-1,0 0 0,1 0 1,-1 1-1,2-1 1,-1 0-1,1 1 0,0-1 1,0 0-1,3 14 0,-3-20-25,1 1 0,-1-1 0,1 0 0,0 1 1,0-1-1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1-1 0,0 1 0,1-1 0,-1 0 1,1 1-1,-1-1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1-1 0,3 0 0,-1 1-8,0-1 0,1 0 0,-1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0-1,3-3 1,-2 1 42,0 0 0,0 0-1,-1-1 1,1 1 0,-1-1-1,0 0 1,2-8 0,-4 12 62,1 3-88,1-1 1,0 1-1,-1 0 0,0-1 0,1 1 1,-1 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,1 3 0,8 15 28,-8-17-52,1 0 0,0-1 0,0 1-1,0 0 1,0-1 0,1 0 0,-1 0 0,1 0-1,-1 0 1,1-1 0,0 1 0,0-1-1,0 0 1,0 0 0,-1 0 0,7 0-1,-8-1-35,1 0-1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 1,0-1-1,0 0 0,0 0 0,0 1 0,0-1 0,-1-1 0,1 1 1,0 0-1,-1-1 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 0 1,0 0-1,3-4 0,-2 0-23,1 1 1,-1-1-1,0 0 0,0 0 1,-1-1-1,0 1 1,0 0-1,0-1 0,-1 1 1,0-1-1,0 0 1,-1-13 650,0 38-271,0 3-67,-1-8-120,1 0 0,0 0 1,1 0-1,5 23 0,-6-33-128,1 0 1,0-1 0,0 1-1,0-1 1,0 1-1,0-1 1,1 1-1,-1-1 1,1 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0-1-1,1 1 1,-1-1-1,1 0 1,-1 1-1,1-1 1,-1 0-1,1-1 1,-1 1-1,1 0 1,0-1-1,-1 1 1,4-1-1,-3 0-117,4 1-574,-1-1 0,1 0 0,0 0 0,-1-1 0,11-1-1,10-11-4803</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1215.82">1057 65 3025,'0'0'1041</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1440.08">1057 78 7027,'119'-21'5715,"-119"30"-5203,0 19-96,0 9 673,5 2-673,0 5-176,6-5-176,0 4-48,0-3-16,5 0-928,5-3-1137,6-9-817,5-10 225,6-12 1072</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2179.36">1662 293 1713,'0'0'10485,"-12"-11"-9066,-40-36-440,49 45-918,0 0 0,0 0 0,-1 0 0,1 1 0,0 0 1,-1-1-1,1 1 0,-1 1 0,1-1 0,-1 0 0,0 1 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 1 1,0-1-1,1 1 0,-1 0 0,1 0 0,-1 0 0,1 1 0,0-1 0,-1 1 0,-4 3 0,0 0 12,0 1 0,1 0-1,-1 0 1,1 1-1,1-1 1,-1 2-1,-8 12 1,13-17-72,0 0 0,1 0-1,0 0 1,-1 1 0,1-1 0,0 0 0,0 1 0,1-1-1,-1 1 1,1-1 0,0 1 0,0-1 0,0 5-1,0-4-22,1-3-35,0 0 0,-1 0 0,1 0 0,0 0 0,0-1-1,0 1 1,-1 0 0,1-1 0,0 1 0,0 0 0,0-1-1,0 1 1,0-1 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 0-1,0 1 1,0-1 0,0 0 0,0 0 0,0 0 0,1-1-1,-1 1 1,1 0 0,35-2-982,-32 1 980,0 0 0,0-1 0,0 1 0,0-1 0,0 0 0,0-1 0,-1 1 0,1-1 0,-1 0 0,1 0 0,3-4 0,21-14 49,-28 21 656,11 40 413,-10-36-1038,0 1 1,1-1-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,1-1-1,-1 1 0,1-1 1,0 0-1,0 0 1,0-1-1,9 5 1,-11-6-13,0 0 1,1 0 0,-1-1-1,1 1 1,-1-1 0,0 1-1,1-1 1,-1 0 0,1 0-1,-1 0 1,1 0 0,-1-1-1,1 1 1,-1 0 0,1-1-1,-1 0 1,0 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,0 0-1,0-1 1,0 1 0,0-1-1,0 1 1,0-1 0,-1 0-1,1 0 1,2-3 0,2-6 6,0 0 1,0 0-1,-1-1 1,-1 0 0,0 0-1,0 0 1,-1 0 0,-1 0-1,2-16 1,0-85 1119,-4 105-590,-2 56-570,1-29 36,0 0-1,1 0 0,5 37 1,-4-54-26,0-1 0,-1 1 0,1-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 0 0,2 0 0,52 1-504,-39-2 367,4 1-20,-14-1 29,1 0 0,0 1 0,0 1 0,-1-1-1,1 1 1,0 0 0,-1 1 0,1 0 0,-1 0 0,12 6 0,-18-8 138,-1 0-1,0 0 1,1 0-1,-1 0 1,0 1-1,1-1 1,-1 0-1,0 0 1,1 0-1,-1 1 1,0-1-1,1 0 1,-1 0-1,0 1 1,0-1-1,1 0 1,-1 1-1,0-1 1,0 0-1,0 1 1,0-1-1,1 0 1,-1 1-1,0-1 1,0 0-1,0 1 1,0-1-1,0 1 1,0-1-1,0 0 1,0 1-1,0-1 1,0 0-1,0 1 1,0-1-1,0 1 1,0-1 0,-1 0-1,1 1 1,0-1-1,0 0 1,0 1-1,0-1 1,-1 0-1,1 0 1,0 1-1,0-1 1,-1 0-1,1 1 1,0-1-1,0 0 1,-1 0-1,1 0 1,0 1-1,-1-1 1,1 0-1,0 0 1,-1 0-1,0 1 1,-23 9 346,21-9-335,-124 32 807,37-11-1585,88-22-939,2-9-7761</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2395.82">2081 1 5507,'0'0'10420,"27"150"-9779,-21-104-385,-1 4-128,6-1-128,-1 0-144,7-6-1841,9-6-2449,7-19-2962</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2673.25">2310 311 8404,'0'0'5493,"13"-15"-5325,65-72 27,-76 86-150,-1-1 0,1 0 0,-1 0-1,1 0 1,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,-1 1-1,1 0 1,-1-1 0,0 1 0,1 0 0,-1-1 0,0-2 0,-1 3 2,1 1 0,0 0 0,-1-1 0,1 1 0,-1 0 1,1 0-1,-1-1 0,0 1 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,-1 0 1,1 1-1,0-1 0,0 0 0,-1 1 0,1 0 0,0-1 0,-1 1 0,1 0 1,0 0-1,-1 0 0,-1 0 0,-3-1-18,0 1 0,0 0 0,0 0 0,0 0 0,0 1 0,0 0 0,1 0-1,-1 1 1,0 0 0,1-1 0,-1 2 0,1-1 0,-1 1 0,1 0 0,0 0 0,0 0 0,0 1 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 1 0,1-1 0,-1 1 0,1 0-1,0 0 1,0 1 0,1-1 0,-1 0 0,1 1 0,0 0 0,-1 8 0,0-4-25,0 1 0,1-1 0,0 1 0,1-1 0,0 1 0,2 19 0,-1-25-127,1-1-1,0 0 1,-1 0 0,2 1 0,-1-1 0,0 0 0,1 0-1,0 0 1,0 0 0,0-1 0,0 1 0,1-1 0,-1 1-1,1-1 1,0 0 0,0 0 0,0 0 0,1 0-1,6 4 1,44 17-3062,17-7-1791</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink3.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2024-12-29T17:24:37.594"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-      <inkml:brushProperty name="color" value="#004F8B"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">19 298 1953,'0'0'7297,"-5"-2"-6609,-9-9 247,21 7 1108,36 7 900,-26-1-3792,402 23 1190,-349-19-418,-70-8 85,0 0 1,0 1-1,0-1 1,0 1-1,0-1 1,0 0-1,0 1 1,0-1-1,-1 1 1,1-1-1,0 0 1,-1 1-1,0-1 1,1 1-1,-3-3 1,-1 0 2,0 0 1,0 0-1,-1 1 0,1-1 1,-1 1-1,0 0 1,0 0-1,0 1 0,-1 0 1,-9-4-1,72 1-1502,-50 5 1462,0 0 0,0 0 0,0 1 0,-1 0 0,1 0-1,10 4 1,-16-5 28,0 1-1,-1-1 1,1 0-1,0 1 1,0-1 0,-1 1-1,1-1 1,0 1-1,0 0 1,-1-1-1,1 1 1,-1-1-1,1 1 1,-1 0-1,1 0 1,-1-1-1,1 1 1,-1 0-1,1 0 1,-1 0-1,0 0 1,1 1-1,-1-1 21,-1 1 0,1 0-1,0 0 1,-1-1 0,1 1-1,-1 0 1,1-1 0,-1 1-1,0 0 1,0-1 0,0 1-1,0-1 1,0 0 0,0 1-1,0-1 1,-2 2 0,-35 32 196,32-30-194,-1 0 0,1 0 0,0 1 0,1 0 0,-10 13 0,13-16-452,0 0 0,1 1 1,0-1-1,-1 0 0,1 1 1,0-1-1,1 1 0,-1-1 1,1 1-1,-1 6 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="561.79">895 191 3185,'0'0'5921,"1"4"-4313,4 38-657,-2-1 0,-5 64 0,1-30-1512,1-74 62,1-7-547,4-57 34,-6 54 1026,1 1 0,0 0 0,1-1-1,-1 1 1,2 0 0,-1-1 0,1 1 0,0 0 0,1 0-1,0 0 1,0 1 0,7-13 0,-8 19 16,1-1 0,-1 1 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 1 0,1-1 0,0 1 0,0 0 1,0 0-1,-1 0 0,6 1 0,38 6 615,-36-2-511,-1 1 1,-1 0-1,1 0 0,-1 0 0,0 1 0,-1 1 0,0-1 0,0 1 0,0 0 0,7 12 0,-6-7-723,2-1-1,-1-1 1,22 19-1,-30-29 276,1 0-1,-1 0 1,1 0 0,0 0-1,-1-1 1,1 1-1,-1-1 1,1 1-1,0-1 1,0 1 0,-1-1-1,1 0 1,2 0-1,2 0-2299</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="832.67">1242 255 560,'0'0'3877,"0"-17"-2685,0-54 38,-2 110 4151,-2 102-5354,4-139-304,1 1 1,-1-1-1,0 0 0,1 1 0,-1-1 1,1 0-1,-1 1 0,1-1 1,0 0-1,0 0 0,0 0 0,0 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1-1 1,0 1-1,0-1 0,0 1 1,0-1-1,4 2 0,10 2-3519</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1177.84">1242 255 1393,'125'2'1827,"-106"-4"513,-20 0-881,0 1-1385,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 1,0 0-1,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 1 1,0 0-1,-2 3 1,1-1 1,1 1 0,-1 0-1,1 0 1,-1 0 0,1 0 0,0 0-1,0 0 1,1 0 0,-1 0-1,1 0 1,0 0 0,0 0-1,0 0 1,1 0 0,0 1 0,1 3-1,-2-5-64,1-1 0,1 0 0,-1 0 0,0 1 0,0-1 0,1 0-1,-1 0 1,1 0 0,0-1 0,-1 1 0,1 0 0,0 0 0,0-1 0,0 0-1,0 1 1,1-1 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,1-1-1,-1 1 1,0-1 0,1 1 0,-1-1 0,1 0 0,3 0 0,-4 0-1,1 0-1,-1 1 1,1-1 0,-1-1 0,1 1 0,0 0 0,-1-1-1,0 1 1,1-1 0,-1 0 0,1 1 0,-1-1 0,0 0 0,1-1-1,-1 1 1,0 0 0,0-1 0,0 1 0,2-2 0,-3-1 93,1 1 1,0 0-1,-1-1 0,0 1 1,0-1-1,0 1 1,0-1-1,-1 0 1,0 1-1,1-1 1,-1 0-1,-1-5 1,1 8-65,-1-1-1,1 1 1,-1 0 0,0-1 0,1 1 0,-1 0 0,0-1 0,0 1 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0-1,0 1 1,0-1 0,-1 0 0,1 1 0,-1-1 0,1 1 0,0-1-1,-1 1 1,1 0 0,-1-1 0,1 1 0,-4 0 0,-43-3-1159,47 3 971,-1 0-1505</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1463.77">1640 0 2817,'0'0'4450,"-6"20"-3497,-2 14-392,1 1 0,2 0 0,-1 49-1,5-72-410,1 0-27,0 0-1,0 0 1,1 0 0,1 0-1,0 0 1,3 11 0,-3-19-115,0 0 1,0 0 0,0 0-1,1-1 1,-1 1 0,1 0-1,0-1 1,0 0 0,0 0-1,0 0 1,1 0 0,-1 0-1,1-1 1,0 1-1,0-1 1,-1 0 0,2 0-1,-1-1 1,0 1 0,5 0-1,3 1-822,1-1-1,-1 0 0,1-1 0,15-1 0,-22-1-1572,-5-7-548</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1603.37">1645 326 2273,'0'0'9060,"-11"-15"-9156,44 9 16,10-3-512,10 3-737,1-4-1408,0 1-1361</inkml:trace>
-</inkml:ink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -40652,7 +40351,7 @@
   <dimension ref="B1:M1000"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -40903,7 +40602,7 @@
         <v>C</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="F14" s="25"/>
       <c r="G14" s="25"/>
@@ -41983,7 +41682,7 @@
   <dimension ref="B1:H1000"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -42072,91 +41771,87 @@
       <c r="D12" s="13"/>
     </row>
     <row r="13" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="13"/>
+      <c r="B13" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="C13" s="12" t="e">
+        <f>10/0</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D13" s="13" t="str">
+        <f>IFERROR(10/0,"Issue with calculation")</f>
+        <v>Issue with calculation</v>
+      </c>
+      <c r="E13">
+        <v>10</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <f>E13/F13</f>
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <f>IFERROR(E13/F13,"Issue")</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="9"/>
-      <c r="E14" s="23" t="s">
-        <v>322</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>321</v>
-      </c>
-      <c r="G14" s="23" t="s">
-        <v>324</v>
-      </c>
-      <c r="H14" s="23" t="s">
-        <v>323</v>
+      <c r="E14" s="23">
+        <v>20</v>
+      </c>
+      <c r="F14" s="23">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ref="G14:G15" si="0">E14/F14</f>
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <f>IFERROR(E14/F14,"Issue")</f>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="9"/>
       <c r="E15">
-        <v>1500</v>
+        <v>30</v>
       </c>
       <c r="F15">
-        <v>5</v>
-      </c>
-      <c r="G15">
-        <f>E15/F15</f>
-        <v>300</v>
-      </c>
-      <c r="H15">
-        <f>IFERROR(E15/F15,"Error While Calculating")</f>
-        <v>300</v>
+        <v>0</v>
+      </c>
+      <c r="G15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H15" t="str">
+        <f>IFERROR(E15/F15,"Issue")</f>
+        <v>Issue</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="9"/>
-      <c r="E16">
-        <v>1000</v>
-      </c>
-      <c r="F16">
-        <v>10</v>
-      </c>
-      <c r="G16">
-        <f t="shared" ref="G16:G17" si="0">E16/F16</f>
-        <v>100</v>
-      </c>
-      <c r="H16">
-        <f>IFERROR(E16/F16,"Error While Calculating")</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="17" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" s="9"/>
-      <c r="E17">
-        <v>5000</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H17" t="str">
-        <f>IFERROR(E17/F17,"Error While Calculating")</f>
-        <v>Error While Calculating</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="19" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="20" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="21" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="22" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="23" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="24" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="25" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="26" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="27" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="28" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="29" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="30" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="31" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="32" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    </row>
+    <row r="18" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="19" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="20" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="21" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="22" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="23" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="24" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="25" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="26" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="27" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="28" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="29" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="30" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="31" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="32" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -43136,8 +42831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B1:E1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -43164,19 +42859,32 @@
       <c r="B4" s="10" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2" t="b">
+        <f>ISERROR(B4)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="10" t="e">
         <v>#N/A</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="39"/>
+      <c r="E5" t="b">
+        <f>ISBLANK(D5)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="10">
         <v>2</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2">
+        <v>2</v>
+      </c>
+      <c r="E6" t="b">
+        <f>ISBLANK(D6)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="10">
@@ -43208,30 +42916,16 @@
     </row>
     <row r="11" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B11" s="6"/>
-      <c r="C11" s="7" t="b">
-        <f>ISBLANK(B3)</f>
-        <v>1</v>
-      </c>
+      <c r="C11" s="7"/>
       <c r="D11" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="E11" t="b">
-        <f>ISBLANK(B5)</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="12" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="6"/>
-      <c r="C12" s="7" t="b">
-        <f>ISERROR(B4)</f>
-        <v>1</v>
-      </c>
+      <c r="C12" s="7"/>
       <c r="D12" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="E12" t="b">
-        <f>ISERROR(B3)</f>
-        <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -43243,6 +42937,10 @@
       <c r="D13" s="8" t="s">
         <v>54</v>
       </c>
+      <c r="E13" t="b">
+        <f>ISNA(B4)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="6"/>
@@ -43253,11 +42951,15 @@
       <c r="D14" s="8" t="s">
         <v>55</v>
       </c>
+      <c r="E14" t="b">
+        <f>ISNUMBER(B8)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="6"/>
       <c r="C15" s="7" t="b">
-        <f>ISODD(B6)</f>
+        <f>ISODD(100)</f>
         <v>0</v>
       </c>
       <c r="D15" s="8" t="s">
@@ -43267,44 +42969,48 @@
     <row r="16" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="6"/>
       <c r="C16" s="7" t="b">
-        <f>ISEVEN(B7)</f>
-        <v>0</v>
+        <f>ISEVEN(100)</f>
+        <v>1</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" s="6"/>
       <c r="C17" s="7" t="b">
-        <f>ISTEXT(B8)</f>
-        <v>1</v>
+        <f>ISTEXT(B6)</f>
+        <v>0</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E17" t="b">
+        <f>ISTEXT(B8)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B18" s="9"/>
     </row>
-    <row r="19" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B19" s="9"/>
     </row>
-    <row r="20" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B20" s="9"/>
     </row>
-    <row r="21" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="22" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="23" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="24" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="25" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="26" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="27" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="28" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="29" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="30" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="31" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="32" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="21" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="22" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="23" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="24" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="25" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="26" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="27" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="28" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="29" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="30" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="31" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="32" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>

</xml_diff>